<commit_message>
Fix db, add users_excel
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,326 +473,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Написать в телеграме</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2025-02-18   18:35:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Тест</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Тест</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Написать в телеграме</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2025-04-03   19:46:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2025-04-03   19:48:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2025-04-08   16:22:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2025-04-08   16:24:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2025-04-08   16:29:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>тест</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2025-04-09   11:35:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1012882762</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>alekseinushtaev</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Алексей</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2025-02-15   23:29:31</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Excel</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>ntc</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2025-04-09   11:37:28</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add repost, fix ecxel google sheets
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,52 +424,203 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>username</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>first_name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>last_name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Время входа в бота</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Как обращаться</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Вопрос</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Контакт</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Время оформления контакта</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Блокировка бота</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1012882762</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>alekseinushtaev</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Алексей</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-04-11   14:25:18</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-04-12   10:54:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1012882762</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>alekseinushtaev</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Алексей</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-04-11   14:25:18</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025-04-12   10:54:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>last_name</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Время входа в бота</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Блокировка бота</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1012882762</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>alekseinushtaev</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Алексей</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-04-11   14:25:18</t>
         </is>
       </c>
     </row>

</xml_diff>